<commit_message>
Update data loading functionality in data_load_mode.py to prioritize user input for enzyme concentration in substrate concentration variation experiments. Enhance error handling for reading enzyme concentration from the calibration results Excel file. Update output files to include normalization results and MM fit results in the Excel export. Modify raw and detailed result CSV files to reflect new data structure.
</commit_message>
<xml_diff>
--- a/convert_to_csv/raw.xlsx
+++ b/convert_to_csv/raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hyacinth1126\protease-simulator-3\convert_to_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44710AE8-E387-486B-B6C8-037C186E06B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04919645-AB21-49E9-B8FD-A0599E44C021}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20820" windowHeight="7845" xr2:uid="{06DE887C-D289-47A0-A687-FB2266CBEDAF}"/>
   </bookViews>
@@ -110,11 +110,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -433,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82AEEC4-7D05-46D8-A69B-2D4965E31F0F}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -559,7 +556,8 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>3130134.0997100002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -568,7 +566,8 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>5335332.6063200003</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -577,7 +576,8 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <v>8691069.4642200004</v>
+        <f ca="1">#REF!-H$3</f>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -585,8 +585,9 @@
       <c r="J3">
         <v>3</v>
       </c>
-      <c r="K3" s="1">
-        <v>11814000</v>
+      <c r="K3">
+        <f ca="1">#REF!-K$3</f>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -594,8 +595,9 @@
       <c r="M3">
         <v>3</v>
       </c>
-      <c r="N3" s="1">
-        <v>12361800</v>
+      <c r="N3">
+        <f ca="1">#REF!-N$3</f>
+        <v>0</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -603,8 +605,9 @@
       <c r="P3">
         <v>3</v>
       </c>
-      <c r="Q3" s="1">
-        <v>14060200</v>
+      <c r="Q3">
+        <f ca="1">#REF!-Q$3</f>
+        <v>0</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -618,7 +621,8 @@
         <v>0.5</v>
       </c>
       <c r="B4">
-        <v>3178073.1976800002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>47939.097970000003</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -627,7 +631,8 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>5520240.5556399999</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>184907.94931999967</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -635,8 +640,9 @@
       <c r="G4">
         <v>3</v>
       </c>
-      <c r="H4" s="1">
-        <v>10156600</v>
+      <c r="H4">
+        <f ca="1">#REF!-H$3</f>
+        <v>1465530.5357799996</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -644,8 +650,9 @@
       <c r="J4">
         <v>3</v>
       </c>
-      <c r="K4" s="1">
-        <v>12683700</v>
+      <c r="K4">
+        <f ca="1">#REF!-K$3</f>
+        <v>869700</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -653,8 +660,9 @@
       <c r="M4">
         <v>3</v>
       </c>
-      <c r="N4" s="1">
-        <v>13231600</v>
+      <c r="N4">
+        <f ca="1">#REF!-N$3</f>
+        <v>869800</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -662,8 +670,9 @@
       <c r="P4">
         <v>3</v>
       </c>
-      <c r="Q4" s="1">
-        <v>14615000</v>
+      <c r="Q4">
+        <f ca="1">#REF!-Q$3</f>
+        <v>554800</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -677,7 +686,8 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>3178073.1976800002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>47939.097970000003</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -686,7 +696,8 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>5520240.5556399999</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>184907.94931999967</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -694,8 +705,9 @@
       <c r="G5">
         <v>3</v>
       </c>
-      <c r="H5" s="1">
-        <v>11259200</v>
+      <c r="H5">
+        <f ca="1">#REF!-H$3</f>
+        <v>2568130.5357799996</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -703,8 +715,9 @@
       <c r="J5">
         <v>3</v>
       </c>
-      <c r="K5" s="1">
-        <v>12916600</v>
+      <c r="K5">
+        <f ca="1">#REF!-K$3</f>
+        <v>1102600</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -712,8 +725,9 @@
       <c r="M5">
         <v>3</v>
       </c>
-      <c r="N5" s="1">
-        <v>13464400</v>
+      <c r="N5">
+        <f ca="1">#REF!-N$3</f>
+        <v>1102600</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -721,8 +735,9 @@
       <c r="P5">
         <v>3</v>
       </c>
-      <c r="Q5" s="1">
-        <v>14751900</v>
+      <c r="Q5">
+        <f ca="1">#REF!-Q$3</f>
+        <v>691700</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -736,7 +751,8 @@
         <v>1.5</v>
       </c>
       <c r="B6">
-        <v>3178073.1976800002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>47939.097970000003</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -745,7 +761,8 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <v>5287393.5083600003</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>-47939.097959999926</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -753,8 +770,9 @@
       <c r="G6">
         <v>3</v>
       </c>
-      <c r="H6" s="1">
-        <v>11950900</v>
+      <c r="H6">
+        <f ca="1">#REF!-H$3</f>
+        <v>3259830.5357799996</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -762,8 +780,9 @@
       <c r="J6">
         <v>3</v>
       </c>
-      <c r="K6" s="1">
-        <v>13005600</v>
+      <c r="K6">
+        <f ca="1">#REF!-K$3</f>
+        <v>1191600</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -771,8 +790,9 @@
       <c r="M6">
         <v>3</v>
       </c>
-      <c r="N6" s="1">
-        <v>13649300</v>
+      <c r="N6">
+        <f ca="1">#REF!-N$3</f>
+        <v>1287500</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -780,8 +800,9 @@
       <c r="P6">
         <v>3</v>
       </c>
-      <c r="Q6" s="1">
-        <v>14888900</v>
+      <c r="Q6">
+        <f ca="1">#REF!-Q$3</f>
+        <v>828700</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -795,7 +816,8 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>3130134.0997100002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -804,7 +826,8 @@
         <v>3</v>
       </c>
       <c r="E7">
-        <v>5335332.6063200003</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -812,8 +835,9 @@
       <c r="G7">
         <v>3</v>
       </c>
-      <c r="H7" s="1">
-        <v>12135800</v>
+      <c r="H7">
+        <f ca="1">#REF!-H$3</f>
+        <v>3444730.5357799996</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -821,8 +845,9 @@
       <c r="J7">
         <v>3</v>
       </c>
-      <c r="K7" s="1">
-        <v>13094600</v>
+      <c r="K7">
+        <f ca="1">#REF!-K$3</f>
+        <v>1280600</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -830,8 +855,9 @@
       <c r="M7">
         <v>3</v>
       </c>
-      <c r="N7" s="1">
-        <v>13786300</v>
+      <c r="N7">
+        <f ca="1">#REF!-N$3</f>
+        <v>1424500</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -839,8 +865,9 @@
       <c r="P7">
         <v>3</v>
       </c>
-      <c r="Q7" s="1">
-        <v>15210800</v>
+      <c r="Q7">
+        <f ca="1">#REF!-Q$3</f>
+        <v>1150600</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -854,7 +881,8 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>3041104.3463400002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>-89029.753370000049</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -863,7 +891,8 @@
         <v>3</v>
       </c>
       <c r="E8">
-        <v>5335332.6063200003</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -871,8 +900,9 @@
       <c r="G8">
         <v>3</v>
       </c>
-      <c r="H8" s="1">
-        <v>12224900</v>
+      <c r="H8">
+        <f ca="1">#REF!-H$3</f>
+        <v>3533830.5357799996</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -880,8 +910,9 @@
       <c r="J8">
         <v>3</v>
       </c>
-      <c r="K8" s="1">
-        <v>12957600</v>
+      <c r="K8">
+        <f ca="1">#REF!-K$3</f>
+        <v>1143600</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -889,8 +920,9 @@
       <c r="M8">
         <v>3</v>
       </c>
-      <c r="N8" s="1">
-        <v>14012300</v>
+      <c r="N8">
+        <f ca="1">#REF!-N$3</f>
+        <v>1650500</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -898,8 +930,9 @@
       <c r="P8">
         <v>3</v>
       </c>
-      <c r="Q8" s="1">
-        <v>15251900</v>
+      <c r="Q8">
+        <f ca="1">#REF!-Q$3</f>
+        <v>1191700</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -913,7 +946,8 @@
         <v>3.5</v>
       </c>
       <c r="B9">
-        <v>3082195.0017400002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>-47939.097970000003</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -922,7 +956,8 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <v>5383271.7042899998</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>47939.097969999537</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -930,8 +965,9 @@
       <c r="G9">
         <v>3</v>
       </c>
-      <c r="H9" s="1">
-        <v>12635800</v>
+      <c r="H9">
+        <f ca="1">#REF!-H$3</f>
+        <v>3944730.5357799996</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -939,8 +975,9 @@
       <c r="J9">
         <v>3</v>
       </c>
-      <c r="K9" s="1">
-        <v>13142600</v>
+      <c r="K9">
+        <f ca="1">#REF!-K$3</f>
+        <v>1328600</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -948,8 +985,9 @@
       <c r="M9">
         <v>3</v>
       </c>
-      <c r="N9" s="1">
-        <v>14334200</v>
+      <c r="N9">
+        <f ca="1">#REF!-N$3</f>
+        <v>1972400</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -957,8 +995,9 @@
       <c r="P9">
         <v>3</v>
       </c>
-      <c r="Q9" s="1">
-        <v>15573800</v>
+      <c r="Q9">
+        <f ca="1">#REF!-Q$3</f>
+        <v>1513600</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -972,7 +1011,8 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>3082195.0017400002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>-47939.097970000003</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -981,7 +1021,8 @@
         <v>3</v>
       </c>
       <c r="E10">
-        <v>5335332.6063200003</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -989,8 +1030,9 @@
       <c r="G10">
         <v>3</v>
       </c>
-      <c r="H10" s="1">
-        <v>12772700</v>
+      <c r="H10">
+        <f ca="1">#REF!-H$3</f>
+        <v>4081630.5357799996</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -998,8 +1040,9 @@
       <c r="J10">
         <v>3</v>
       </c>
-      <c r="K10" s="1">
-        <v>12916600</v>
+      <c r="K10">
+        <f ca="1">#REF!-K$3</f>
+        <v>1102600</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1007,8 +1050,9 @@
       <c r="M10">
         <v>3</v>
       </c>
-      <c r="N10" s="1">
-        <v>14334200</v>
+      <c r="N10">
+        <f ca="1">#REF!-N$3</f>
+        <v>1972400</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1016,8 +1060,9 @@
       <c r="P10">
         <v>3</v>
       </c>
-      <c r="Q10" s="1">
-        <v>15573800</v>
+      <c r="Q10">
+        <f ca="1">#REF!-Q$3</f>
+        <v>1513600</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -1031,7 +1076,8 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>3082195.0017400002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>-47939.097970000003</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1040,7 +1086,8 @@
         <v>3</v>
       </c>
       <c r="E11">
-        <v>5061394.9036400001</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>-273937.7026800001</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1048,8 +1095,9 @@
       <c r="G11">
         <v>3</v>
       </c>
-      <c r="H11" s="1">
-        <v>12916600</v>
+      <c r="H11">
+        <f ca="1">#REF!-H$3</f>
+        <v>4225530.5357799996</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1057,8 +1105,9 @@
       <c r="J11">
         <v>3</v>
       </c>
-      <c r="K11" s="1">
-        <v>11355100</v>
+      <c r="K11">
+        <f ca="1">#REF!-K$3</f>
+        <v>-458900</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1066,8 +1115,9 @@
       <c r="M11">
         <v>3</v>
       </c>
-      <c r="N11" s="1">
-        <v>14888900</v>
+      <c r="N11">
+        <f ca="1">#REF!-N$3</f>
+        <v>2527100</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -1075,8 +1125,9 @@
       <c r="P11">
         <v>3</v>
       </c>
-      <c r="Q11" s="1">
-        <v>15573800</v>
+      <c r="Q11">
+        <f ca="1">#REF!-Q$3</f>
+        <v>1513600</v>
       </c>
       <c r="R11">
         <v>0</v>
@@ -1090,7 +1141,8 @@
         <v>6.5</v>
       </c>
       <c r="B12">
-        <v>3130134.0997100002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1099,7 +1151,8 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>5424362.3596999999</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>89029.75337999966</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1107,8 +1160,9 @@
       <c r="G12">
         <v>3</v>
       </c>
-      <c r="H12" s="1">
-        <v>13053500</v>
+      <c r="H12">
+        <f ca="1">#REF!-H$3</f>
+        <v>4362430.5357799996</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1116,8 +1170,9 @@
       <c r="J12">
         <v>3</v>
       </c>
-      <c r="K12" s="1">
-        <v>12820700</v>
+      <c r="K12">
+        <f ca="1">#REF!-K$3</f>
+        <v>1006700</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1125,8 +1180,9 @@
       <c r="M12">
         <v>3</v>
       </c>
-      <c r="N12" s="1">
-        <v>14615000</v>
+      <c r="N12">
+        <f ca="1">#REF!-N$3</f>
+        <v>2253200</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -1134,8 +1190,9 @@
       <c r="P12">
         <v>3</v>
       </c>
-      <c r="Q12" s="1">
-        <v>15854500</v>
+      <c r="Q12">
+        <f ca="1">#REF!-Q$3</f>
+        <v>1794300</v>
       </c>
       <c r="R12">
         <v>0</v>
@@ -1149,7 +1206,8 @@
         <v>7</v>
       </c>
       <c r="B13">
-        <v>3041104.3463400002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>-89029.753370000049</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1158,7 +1216,8 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <v>5287393.5083600003</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>-47939.097959999926</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1166,8 +1225,9 @@
       <c r="G13">
         <v>3</v>
       </c>
-      <c r="H13" s="1">
-        <v>12820700</v>
+      <c r="H13">
+        <f ca="1">#REF!-H$3</f>
+        <v>4129630.5357799996</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1175,8 +1235,9 @@
       <c r="J13">
         <v>3</v>
       </c>
-      <c r="K13" s="1">
-        <v>12868600</v>
+      <c r="K13">
+        <f ca="1">#REF!-K$3</f>
+        <v>1054600</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1184,8 +1245,9 @@
       <c r="M13">
         <v>3</v>
       </c>
-      <c r="N13" s="1">
-        <v>14615000</v>
+      <c r="N13">
+        <f ca="1">#REF!-N$3</f>
+        <v>2253200</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -1193,8 +1255,9 @@
       <c r="P13">
         <v>3</v>
       </c>
-      <c r="Q13" s="1">
-        <v>15717600</v>
+      <c r="Q13">
+        <f ca="1">#REF!-Q$3</f>
+        <v>1657400</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -1208,7 +1271,8 @@
         <v>7.5</v>
       </c>
       <c r="B14">
-        <v>3082195.0017400002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>-47939.097970000003</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1217,7 +1281,8 @@
         <v>3</v>
       </c>
       <c r="E14">
-        <v>5383271.7042899998</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>47939.097969999537</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1225,8 +1290,9 @@
       <c r="G14">
         <v>3</v>
       </c>
-      <c r="H14" s="1">
-        <v>13053500</v>
+      <c r="H14">
+        <f ca="1">#REF!-H$3</f>
+        <v>4362430.5357799996</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1234,8 +1300,9 @@
       <c r="J14">
         <v>3</v>
       </c>
-      <c r="K14" s="1">
-        <v>13053500</v>
+      <c r="K14">
+        <f ca="1">#REF!-K$3</f>
+        <v>1239500</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1243,8 +1310,9 @@
       <c r="M14">
         <v>3</v>
       </c>
-      <c r="N14" s="1">
-        <v>14841000</v>
+      <c r="N14">
+        <f ca="1">#REF!-N$3</f>
+        <v>2479200</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -1252,8 +1320,9 @@
       <c r="P14">
         <v>3</v>
       </c>
-      <c r="Q14" s="1">
-        <v>16032600</v>
+      <c r="Q14">
+        <f ca="1">#REF!-Q$3</f>
+        <v>1972400</v>
       </c>
       <c r="R14">
         <v>0</v>
@@ -1267,7 +1336,8 @@
         <v>8</v>
       </c>
       <c r="B15">
-        <v>3226012.2956500002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>95878.195940000005</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1276,7 +1346,8 @@
         <v>3</v>
       </c>
       <c r="E15">
-        <v>5424362.3596999999</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>89029.75337999966</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1284,8 +1355,9 @@
       <c r="G15">
         <v>3</v>
       </c>
-      <c r="H15" s="1">
-        <v>13005600</v>
+      <c r="H15">
+        <f ca="1">#REF!-H$3</f>
+        <v>4314530.5357799996</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1293,8 +1365,9 @@
       <c r="J15">
         <v>3</v>
       </c>
-      <c r="K15" s="1">
-        <v>12957600</v>
+      <c r="K15">
+        <f ca="1">#REF!-K$3</f>
+        <v>1143600</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1302,8 +1375,9 @@
       <c r="M15">
         <v>3</v>
       </c>
-      <c r="N15" s="1">
-        <v>14936800</v>
+      <c r="N15">
+        <f ca="1">#REF!-N$3</f>
+        <v>2575000</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -1311,8 +1385,9 @@
       <c r="P15">
         <v>3</v>
       </c>
-      <c r="Q15" s="1">
-        <v>15895600</v>
+      <c r="Q15">
+        <f ca="1">#REF!-Q$3</f>
+        <v>1835400</v>
       </c>
       <c r="R15">
         <v>0</v>
@@ -1326,7 +1401,8 @@
         <v>10</v>
       </c>
       <c r="B16">
-        <v>3041104.3463400002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>-89029.753370000049</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1335,7 +1411,8 @@
         <v>3</v>
       </c>
       <c r="E16">
-        <v>5472301.4576700004</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>136968.85135000013</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1343,8 +1420,9 @@
       <c r="G16">
         <v>3</v>
       </c>
-      <c r="H16" s="1">
-        <v>13005600</v>
+      <c r="H16">
+        <f ca="1">#REF!-H$3</f>
+        <v>4314530.5357799996</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1352,8 +1430,9 @@
       <c r="J16">
         <v>3</v>
       </c>
-      <c r="K16" s="1">
-        <v>13142600</v>
+      <c r="K16">
+        <f ca="1">#REF!-K$3</f>
+        <v>1328600</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -1361,8 +1440,9 @@
       <c r="M16">
         <v>3</v>
       </c>
-      <c r="N16" s="1">
-        <v>15162800</v>
+      <c r="N16">
+        <f ca="1">#REF!-N$3</f>
+        <v>2801000</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -1370,8 +1450,9 @@
       <c r="P16">
         <v>3</v>
       </c>
-      <c r="Q16" s="1">
-        <v>16080500</v>
+      <c r="Q16">
+        <f ca="1">#REF!-Q$3</f>
+        <v>2020300</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -1385,7 +1466,8 @@
         <v>12</v>
       </c>
       <c r="B17">
-        <v>3082195.0017400002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>-47939.097970000003</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1394,7 +1476,8 @@
         <v>3</v>
       </c>
       <c r="E17">
-        <v>5657209.4069800004</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>321876.80066000018</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1402,8 +1485,9 @@
       <c r="G17">
         <v>3</v>
       </c>
-      <c r="H17" s="1">
-        <v>13553500</v>
+      <c r="H17">
+        <f ca="1">#REF!-H$3</f>
+        <v>4862430.5357799996</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1411,8 +1495,9 @@
       <c r="J17">
         <v>3</v>
       </c>
-      <c r="K17" s="1">
-        <v>12957600</v>
+      <c r="K17">
+        <f ca="1">#REF!-K$3</f>
+        <v>1143600</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1420,8 +1505,9 @@
       <c r="M17">
         <v>3</v>
       </c>
-      <c r="N17" s="1">
-        <v>15162800</v>
+      <c r="N17">
+        <f ca="1">#REF!-N$3</f>
+        <v>2801000</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1429,8 +1515,9 @@
       <c r="P17">
         <v>3</v>
       </c>
-      <c r="Q17" s="1">
-        <v>16128500</v>
+      <c r="Q17">
+        <f ca="1">#REF!-Q$3</f>
+        <v>2068300</v>
       </c>
       <c r="R17">
         <v>0</v>
@@ -1444,7 +1531,8 @@
         <v>14</v>
       </c>
       <c r="B18">
-        <v>3082195.0017400002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>-47939.097970000003</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1453,7 +1541,8 @@
         <v>3</v>
       </c>
       <c r="E18">
-        <v>5424362.3596999999</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>89029.75337999966</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1461,8 +1550,9 @@
       <c r="G18">
         <v>3</v>
       </c>
-      <c r="H18" s="1">
-        <v>13375400</v>
+      <c r="H18">
+        <f ca="1">#REF!-H$3</f>
+        <v>4684330.5357799996</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1470,8 +1560,9 @@
       <c r="J18">
         <v>3</v>
       </c>
-      <c r="K18" s="1">
-        <v>12916600</v>
+      <c r="K18">
+        <f ca="1">#REF!-K$3</f>
+        <v>1102600</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1479,8 +1570,9 @@
       <c r="M18">
         <v>3</v>
       </c>
-      <c r="N18" s="1">
-        <v>15162800</v>
+      <c r="N18">
+        <f ca="1">#REF!-N$3</f>
+        <v>2801000</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1488,8 +1580,9 @@
       <c r="P18">
         <v>3</v>
       </c>
-      <c r="Q18" s="1">
-        <v>16313400</v>
+      <c r="Q18">
+        <f ca="1">#REF!-Q$3</f>
+        <v>2253200</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -1503,7 +1596,8 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>3226012.2956500002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>95878.195940000005</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1512,7 +1606,8 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <v>5705148.50495</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>369815.89862999972</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1520,8 +1615,9 @@
       <c r="G19">
         <v>3</v>
       </c>
-      <c r="H19" s="1">
-        <v>13649300</v>
+      <c r="H19">
+        <f ca="1">#REF!-H$3</f>
+        <v>4958230.5357799996</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -1529,8 +1625,9 @@
       <c r="J19">
         <v>3</v>
       </c>
-      <c r="K19" s="1">
-        <v>13697300</v>
+      <c r="K19">
+        <f ca="1">#REF!-K$3</f>
+        <v>1883300</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -1538,8 +1635,9 @@
       <c r="M19">
         <v>3</v>
       </c>
-      <c r="N19" s="1">
-        <v>15806600</v>
+      <c r="N19">
+        <f ca="1">#REF!-N$3</f>
+        <v>3444800</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1547,8 +1645,9 @@
       <c r="P19">
         <v>3</v>
       </c>
-      <c r="Q19" s="1">
-        <v>16676400</v>
+      <c r="Q19">
+        <f ca="1">#REF!-Q$3</f>
+        <v>2616200</v>
       </c>
       <c r="R19">
         <v>0</v>
@@ -1562,7 +1661,8 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>3130134.0997100002</v>
+        <f ca="1">#REF!-B$3</f>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1571,7 +1671,8 @@
         <v>3</v>
       </c>
       <c r="E20">
-        <v>5472301.4576700004</v>
+        <f ca="1">#REF!-E$3</f>
+        <v>136968.85135000013</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1579,8 +1680,9 @@
       <c r="G20">
         <v>3</v>
       </c>
-      <c r="H20" s="1">
-        <v>13512400</v>
+      <c r="H20">
+        <f ca="1">#REF!-H$3</f>
+        <v>4821330.5357799996</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1588,8 +1690,9 @@
       <c r="J20">
         <v>3</v>
       </c>
-      <c r="K20" s="1">
-        <v>13416500</v>
+      <c r="K20">
+        <f ca="1">#REF!-K$3</f>
+        <v>1602500</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -1597,8 +1700,9 @@
       <c r="M20">
         <v>3</v>
       </c>
-      <c r="N20" s="1">
-        <v>15395700</v>
+      <c r="N20">
+        <f ca="1">#REF!-N$3</f>
+        <v>3033900</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1606,8 +1710,9 @@
       <c r="P20">
         <v>3</v>
       </c>
-      <c r="Q20" s="1">
-        <v>16628400</v>
+      <c r="Q20">
+        <f ca="1">#REF!-Q$3</f>
+        <v>2568200</v>
       </c>
       <c r="R20">
         <v>0</v>

</xml_diff>